<commit_message>
Added the search and delete for a specific patient
</commit_message>
<xml_diff>
--- a/clinic_data.xlsx
+++ b/clinic_data.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Name</t>
   </si>
@@ -26,16 +26,19 @@
     <t>Disease</t>
   </si>
   <si>
+    <t>Doctor</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Time Slot</t>
+  </si>
+  <si>
     <t>Mahmoud</t>
   </si>
   <si>
     <t>Male</t>
-  </si>
-  <si>
-    <t>Osteogenesis</t>
-  </si>
-  <si>
-    <t>Hesham</t>
   </si>
   <si>
     <t>Headache</t>
@@ -83,7 +86,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -102,33 +105,28 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B2" t="n">
         <v>31.0</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" t="n">
-        <v>28.0</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>